<commit_message>
up fonctionnal without remove page
</commit_message>
<xml_diff>
--- a/test_fr.xlsx
+++ b/test_fr.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,7 +434,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Haute</t>
+          <t>Haute PAGE 32 OF  33</t>
         </is>
       </c>
     </row>
@@ -654,6 +654,57 @@
         </is>
       </c>
       <c r="C14" t="inlineStr">
+        <is>
+          <t>Informations</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Potential Usage of Vulnerable Log4J</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Informations</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Potential Usage of Vulnerable Log4J</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Informations</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Potential Usage of Vulnerable Log4J</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
         <is>
           <t>Informations</t>
         </is>

</xml_diff>